<commit_message>
add a cetificate sheet
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="experience" sheetId="1" r:id="rId1"/>
     <sheet name="education" sheetId="2" r:id="rId2"/>
+    <sheet name="cetificate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="1379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3714" uniqueCount="1390">
   <si>
     <t>name</t>
   </si>
@@ -4152,6 +4153,39 @@
   </si>
   <si>
     <t>2012</t>
+  </si>
+  <si>
+    <t>cetificate</t>
+  </si>
+  <si>
+    <t>Jan Thede</t>
+  </si>
+  <si>
+    <t>Jeanine Casey</t>
+  </si>
+  <si>
+    <t>Jeff Bakalar</t>
+  </si>
+  <si>
+    <t>Jill Fedoruk</t>
+  </si>
+  <si>
+    <t>金伟煌</t>
+  </si>
+  <si>
+    <t>John Wain</t>
+  </si>
+  <si>
+    <t>Joseph Sullivan</t>
+  </si>
+  <si>
+    <t>CPA</t>
+  </si>
+  <si>
+    <t>CPA, CFA</t>
+  </si>
+  <si>
+    <t>CFA</t>
   </si>
 </sst>
 </file>
@@ -18931,4 +18965,935 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C111"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>